<commit_message>
Updated mitre ttp mapping
</commit_message>
<xml_diff>
--- a/mitre_ttp_mapping/Zeek-Agent_Evaluation.xlsx
+++ b/mitre_ttp_mapping/Zeek-Agent_Evaluation.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jojo\Desktop\SecurityLab\zeek-agent\mitre_ttp_mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B257ED98-D15C-4F40-9770-B22C327515BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A0DBC5-E010-47FA-B5F9-B272CE534745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C89A58F5-9484-469A-8F93-A65B0037292C}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{C89A58F5-9484-469A-8F93-A65B0037292C}"/>
   </bookViews>
   <sheets>
     <sheet name="Candidate TTPs" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Candidate TTPs'!$A$7:$Q$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Candidate TTPs'!$A$7:$P$7</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="187">
   <si>
     <t>Zeek-Agent Evaluation</t>
   </si>
@@ -100,9 +100,6 @@
   </si>
   <si>
     <t>Other resources</t>
-  </si>
-  <si>
-    <t>Atomic Test available?</t>
   </si>
   <si>
     <t>Link</t>
@@ -156,9 +153,6 @@
     <t>MHR hash submission script</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
     <t>T1566.001 - Spearphishing Attachment</t>
   </si>
   <si>
@@ -181,10 +175,6 @@
 Process CMD Line</t>
   </si>
   <si>
-    <t>4657
-Windows Registry</t>
-  </si>
-  <si>
     <t>7045
 New Service</t>
   </si>
@@ -246,10 +236,6 @@
     <t>External Remote Services</t>
   </si>
   <si>
-    <t>4624
-Authentication logs</t>
-  </si>
-  <si>
     <t>API monitoring</t>
   </si>
   <si>
@@ -390,10 +376,6 @@
   </si>
   <si>
     <t>Credentials in Files</t>
-  </si>
-  <si>
-    <t>file_monitoring
-process_creation</t>
   </si>
   <si>
     <t>conn.log
@@ -614,6 +596,61 @@
   </si>
   <si>
     <t>Detection Comments</t>
+  </si>
+  <si>
+    <t>process_creation
+obj_access_attempt
+network_conn</t>
+  </si>
+  <si>
+    <t>process_creation
+regval_modified</t>
+  </si>
+  <si>
+    <t>process_creation
+network_conn</t>
+  </si>
+  <si>
+    <t>process_creation
+regval_modified
+obj_access_attempt</t>
+  </si>
+  <si>
+    <t>4624
+Account logon</t>
+  </si>
+  <si>
+    <t>account_logon
+network_conn</t>
+  </si>
+  <si>
+    <t>4657
+Registry value modified</t>
+  </si>
+  <si>
+    <t>process_creation
+process_termination
+regval_modified
+obj_access_attempt</t>
+  </si>
+  <si>
+    <t>process_creation
+network_conn
+account_logon</t>
+  </si>
+  <si>
+    <t>process_creation
+obj_access_attempt</t>
+  </si>
+  <si>
+    <t>process_creation
+obj_access_attempt
+regval_modified</t>
+  </si>
+  <si>
+    <t>process_creation
+process_termination
+regval_modified</t>
   </si>
 </sst>
 </file>
@@ -791,7 +828,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -877,6 +914,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1214,11 +1254,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1236AE1C-53F9-4736-A741-4EB0B1B59944}">
-  <dimension ref="A1:S42"/>
+  <dimension ref="A1:R42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S7" sqref="S7"/>
+      <selection pane="bottomLeft" activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -1237,41 +1277,39 @@
     <col min="13" max="13" width="22.33203125" style="20" customWidth="1"/>
     <col min="14" max="14" width="18.6640625" style="20" customWidth="1"/>
     <col min="15" max="16" width="25.6640625" customWidth="1"/>
-    <col min="17" max="17" width="22.6640625" style="20" customWidth="1"/>
-    <col min="18" max="18" width="17" style="19" customWidth="1"/>
-    <col min="19" max="19" width="32" style="19" customWidth="1"/>
+    <col min="17" max="17" width="20.5546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="32" style="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="6" customFormat="1" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:18" s="6" customFormat="1" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
       <c r="E1" s="1"/>
       <c r="F1" s="2"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
-      <c r="Q1" s="5"/>
+      <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-    </row>
-    <row r="2" spans="1:19" s="6" customFormat="1" ht="28.95" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A2" s="35" t="s">
+    </row>
+    <row r="2" spans="1:18" s="6" customFormat="1" ht="28.95" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
       <c r="F2" s="2"/>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
@@ -1281,69 +1319,64 @@
       <c r="L2" s="8"/>
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
-      <c r="Q2" s="5"/>
+      <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-    </row>
-    <row r="3" spans="1:19" s="6" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:18" s="6" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
       <c r="B3" s="3"/>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
-      <c r="Q3" s="5"/>
+      <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
-    </row>
-    <row r="4" spans="1:19" s="11" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:18" s="11" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9"/>
       <c r="B4" s="10"/>
       <c r="M4" s="9"/>
       <c r="N4" s="9"/>
-      <c r="Q4" s="9"/>
+      <c r="Q4" s="12"/>
       <c r="R4" s="12"/>
-      <c r="S4" s="12"/>
-    </row>
-    <row r="5" spans="1:19" s="6" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:18" s="6" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
       <c r="B5" s="3"/>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
-      <c r="Q5" s="5"/>
+      <c r="Q5" s="4"/>
       <c r="R5" s="4"/>
-      <c r="S5" s="4"/>
-    </row>
-    <row r="6" spans="1:19" s="6" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="36" t="s">
+    </row>
+    <row r="6" spans="1:18" s="6" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="36"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="37" t="s">
+      <c r="B6" s="37"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="37"/>
-      <c r="K6" s="37"/>
-      <c r="L6" s="37"/>
-      <c r="M6" s="38" t="s">
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="38"/>
+      <c r="K6" s="38"/>
+      <c r="L6" s="38"/>
+      <c r="M6" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="N6" s="38"/>
-      <c r="O6" s="38"/>
+      <c r="N6" s="39"/>
+      <c r="O6" s="39"/>
       <c r="P6" s="13"/>
       <c r="Q6" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="R6" s="31"/>
-      <c r="S6" s="14" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R6" s="14" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
         <v>6</v>
       </c>
@@ -1380,1009 +1413,980 @@
       <c r="L7" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="M7" s="17" t="s">
+      <c r="M7" s="32" t="s">
         <v>18</v>
       </c>
       <c r="N7" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="O7" s="32" t="s">
+      <c r="O7" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="P7" s="32"/>
+      <c r="P7" s="33"/>
       <c r="Q7" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="R7" s="18" t="s">
+    </row>
+    <row r="8" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="20" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="20" t="s">
+      <c r="B8" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="C8" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="D8" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="E8" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="F8" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="22" t="s">
+      <c r="G8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="G8" s="22" t="s">
+      <c r="H8" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="H8" s="23" t="s">
+      <c r="I8" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="I8" s="21" t="s">
+      <c r="J8" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="J8" s="21" t="s">
+      <c r="K8" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="K8" s="21" t="s">
+      <c r="L8" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="L8" s="21" t="s">
+      <c r="M8" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="N8" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="M8" s="21"/>
-      <c r="N8" s="21" t="s">
+      <c r="O8" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="O8" s="24" t="s">
+      <c r="P8" s="24"/>
+      <c r="Q8" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="P8" s="24"/>
-      <c r="Q8" s="20" t="s">
+    </row>
+    <row r="9" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="R8" s="25" t="s">
+      <c r="B9" s="21" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="20" t="s">
+      <c r="C9" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="D9" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="E9" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="F9" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="G9" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" s="23" t="s">
+        <v>181</v>
+      </c>
+      <c r="I9" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="F9" s="23" t="s">
+      <c r="J9" s="23" t="s">
         <v>44</v>
-      </c>
-      <c r="G9" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="H9" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="I9" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="J9" s="23" t="s">
-        <v>47</v>
       </c>
       <c r="K9" s="21"/>
       <c r="L9" s="21"/>
-      <c r="M9" s="21"/>
+      <c r="M9" s="21" t="s">
+        <v>176</v>
+      </c>
       <c r="N9" s="21"/>
-      <c r="Q9" s="20" t="s">
+      <c r="Q9" s="25" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="R9" s="25" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="20" t="s">
-        <v>39</v>
-      </c>
       <c r="B10" s="21" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E10" s="21"/>
       <c r="F10" s="23" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G10" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H10" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I10" s="26" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="J10" s="21"/>
       <c r="K10" s="21"/>
       <c r="L10" s="21"/>
-      <c r="M10"/>
+      <c r="M10" s="21" t="s">
+        <v>177</v>
+      </c>
       <c r="N10" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q10" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="R10" s="19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="Q10" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="R10" s="25" t="s">
+      <c r="B11" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="S10" s="19" t="s">
+      <c r="C11" s="21" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="20" t="s">
+      <c r="D11" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="E11" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="F11" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="D11" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="E11" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="F11" s="27" t="s">
+      <c r="H11" s="27" t="s">
+        <v>181</v>
+      </c>
+      <c r="I11" s="27" t="s">
         <v>28</v>
-      </c>
-      <c r="G11" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="H11" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="I11" s="27" t="s">
-        <v>29</v>
       </c>
       <c r="J11" s="21"/>
       <c r="K11" s="21"/>
       <c r="L11" s="21"/>
-      <c r="M11"/>
+      <c r="M11" s="21" t="s">
+        <v>178</v>
+      </c>
       <c r="N11" s="21"/>
       <c r="O11" s="28"/>
       <c r="P11" s="28"/>
-      <c r="Q11" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="R11" s="25" t="s">
+      <c r="Q11" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="R11" s="19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="21" t="s">
         <v>61</v>
-      </c>
-      <c r="S11" s="19" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="B12" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="D12" s="21" t="s">
-        <v>64</v>
       </c>
       <c r="E12" s="21"/>
       <c r="F12" s="27" t="s">
-        <v>65</v>
+        <v>179</v>
       </c>
       <c r="G12" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H12" s="21" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="I12" s="21"/>
       <c r="J12" s="21"/>
       <c r="K12" s="21"/>
       <c r="L12" s="21"/>
-      <c r="M12"/>
+      <c r="M12" s="21" t="s">
+        <v>180</v>
+      </c>
       <c r="N12" s="21" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="O12" s="19"/>
       <c r="P12" s="19"/>
-      <c r="Q12" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="R12" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="S12" s="19" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="Q12" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="R12" s="19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E13" s="21"/>
       <c r="F13" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="H13" s="27" t="s">
+        <v>181</v>
+      </c>
+      <c r="I13" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="G13" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="H13" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="I13" s="27" t="s">
-        <v>29</v>
-      </c>
       <c r="J13" s="21" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="K13" s="21"/>
       <c r="L13" s="21"/>
-      <c r="M13"/>
+      <c r="M13" s="21" t="s">
+        <v>178</v>
+      </c>
       <c r="N13" s="21"/>
       <c r="O13" s="28"/>
       <c r="P13" s="28"/>
-      <c r="Q13" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="R13" s="25" t="s">
+      <c r="Q13" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="R13" s="19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="S13" s="19" t="s">
+      <c r="D14" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="21" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="20" t="s">
+      <c r="F14" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="H14" s="23" t="s">
+        <v>181</v>
+      </c>
+      <c r="I14" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="J14" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="B14" s="21" t="s">
+      <c r="K14" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="C14" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="D14" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="E14" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="F14" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="G14" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="H14" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="I14" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="J14" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="K14" s="26" t="s">
-        <v>78</v>
-      </c>
       <c r="L14" s="21"/>
-      <c r="M14"/>
+      <c r="M14" s="21" t="s">
+        <v>178</v>
+      </c>
       <c r="N14" s="21"/>
       <c r="O14" s="28"/>
       <c r="P14" s="28"/>
-      <c r="Q14" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="R14" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="S14" s="19" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="Q14" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="R14" s="19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E15" s="21"/>
       <c r="F15" s="23" t="s">
-        <v>45</v>
+        <v>181</v>
       </c>
       <c r="G15" s="23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H15" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="I15" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="J15" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="K15" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="L15" s="21"/>
+      <c r="M15" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="Q15" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="R15" s="19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="G16" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="H16" s="23" t="s">
+        <v>181</v>
+      </c>
+      <c r="I16" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="I15" s="26" t="s">
+      <c r="J16" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="K16" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="L16" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="M16" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="N16" s="21"/>
+      <c r="Q16" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="R16" s="19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="J15" s="26" t="s">
-        <v>83</v>
-      </c>
-      <c r="K15" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="L15" s="21"/>
-      <c r="M15" s="21"/>
-      <c r="Q15" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="R15" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="S15" s="19" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="B16" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="C16" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="D16" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="E16" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="F16" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="G16" s="23" t="s">
+      <c r="C17" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="H16" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="I16" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="J16" s="23" t="s">
+      <c r="D17" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="K16" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="L16" s="26" t="s">
+      <c r="E17" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="M16" s="21"/>
-      <c r="N16" s="21"/>
-      <c r="Q16" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="R16" s="25" t="s">
+      <c r="F17" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="G17" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="H17" s="23" t="s">
+        <v>181</v>
+      </c>
+      <c r="I17" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="J17" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="K17" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="S16" s="19" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="B17" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="C17" s="21" t="s">
+      <c r="L17" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="M17" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="N17" s="21"/>
+      <c r="Q17" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="D17" s="21" t="s">
+      <c r="R17" s="19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" ht="79.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="E17" s="21" t="s">
+      <c r="B18" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="F17" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="G17" s="23" t="s">
+      <c r="C18" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="F18" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="N18" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="O18" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="P18" s="25"/>
+      <c r="Q18" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="R18" s="19" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="E19" t="s">
+        <v>107</v>
+      </c>
+      <c r="F19" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="H17" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="I17" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="J17" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="K17" s="26" t="s">
-        <v>97</v>
-      </c>
-      <c r="L17" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="M17" s="21"/>
-      <c r="N17" s="21"/>
-      <c r="Q17" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="R17" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="S17" s="19" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" ht="79.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="B18" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="C18" s="21" t="s">
-        <v>101</v>
-      </c>
-      <c r="D18" s="21" t="s">
-        <v>102</v>
-      </c>
-      <c r="E18" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="F18" s="27" t="s">
-        <v>104</v>
-      </c>
-      <c r="N18" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="O18" s="25" t="s">
-        <v>106</v>
-      </c>
-      <c r="P18" s="25"/>
-      <c r="Q18" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="R18" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="S18" s="19" t="s">
+      <c r="G19" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="M19" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="N19" s="21" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="19" spans="1:19" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="B19" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="C19" s="21" t="s">
+      <c r="Q19" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="D19" s="21" t="s">
+      <c r="R19" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="E19" t="s">
+    </row>
+    <row r="20" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="F19" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="G19" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="M19" s="21" t="s">
+      <c r="B20" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="N19" s="21" t="s">
+      <c r="C20" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="Q19" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="R19" s="25" t="s">
+      <c r="D20" s="21" t="s">
         <v>114</v>
-      </c>
-      <c r="S19" s="19" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="B20" s="21" t="s">
-        <v>117</v>
-      </c>
-      <c r="C20" s="21" t="s">
-        <v>118</v>
-      </c>
-      <c r="D20" s="21" t="s">
-        <v>119</v>
       </c>
       <c r="E20" s="21"/>
       <c r="F20" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G20" s="23" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H20" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I20" s="23" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="J20" s="26" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="K20" s="21"/>
       <c r="L20" s="21"/>
-      <c r="M20" s="21"/>
+      <c r="M20" s="21" t="s">
+        <v>177</v>
+      </c>
       <c r="N20" s="21" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="O20" s="29" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="P20" s="29"/>
-      <c r="Q20" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="R20" s="25" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="Q20" s="25" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E21" s="21"/>
       <c r="F21" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G21" s="23" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H21" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I21" s="26" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="J21" s="21"/>
       <c r="K21" s="21"/>
       <c r="L21" s="21"/>
-      <c r="M21"/>
+      <c r="M21" s="21" t="s">
+        <v>177</v>
+      </c>
       <c r="N21" s="21" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="O21" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="P21" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q21" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="P21" s="29" t="s">
+    </row>
+    <row r="22" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="B22" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="D22" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="Q21" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="R21" s="25" t="s">
+      <c r="E22" s="21" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="22" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A22" s="20" t="s">
+      <c r="F22" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="B22" s="21" t="s">
-        <v>130</v>
-      </c>
-      <c r="C22" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="D22" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="E22" s="21" t="s">
-        <v>133</v>
-      </c>
-      <c r="F22" s="27" t="s">
-        <v>134</v>
-      </c>
       <c r="G22" s="27" t="s">
-        <v>65</v>
+        <v>179</v>
       </c>
       <c r="H22" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I22" s="21" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="J22" s="21"/>
       <c r="K22" s="21"/>
       <c r="L22" s="21"/>
-      <c r="M22" s="21"/>
+      <c r="M22" s="21" t="s">
+        <v>183</v>
+      </c>
       <c r="N22" s="21" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="O22" s="25" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="P22" s="24" t="s">
-        <v>136</v>
-      </c>
-      <c r="Q22" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="R22" s="25" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+        <v>131</v>
+      </c>
+      <c r="Q22" s="25" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="20" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E23" s="21" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="F23" s="27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G23" s="27" t="s">
-        <v>65</v>
+        <v>179</v>
       </c>
       <c r="H23" s="27" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I23" s="27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J23" s="21"/>
       <c r="K23" s="21"/>
       <c r="L23" s="21"/>
-      <c r="M23" s="21"/>
+      <c r="M23" s="21" t="s">
+        <v>183</v>
+      </c>
       <c r="N23" s="21" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="O23" s="30" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="P23" s="30"/>
-      <c r="Q23" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="R23" s="25" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="Q23" s="25" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="20" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D24" s="21" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="E24" s="21"/>
       <c r="F24" s="27" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G24" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H24" s="21" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="I24" s="21"/>
       <c r="J24" s="21"/>
       <c r="K24" s="21"/>
       <c r="L24" s="21"/>
-      <c r="M24" s="21"/>
+      <c r="M24" s="21" t="s">
+        <v>184</v>
+      </c>
       <c r="N24" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="O24" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="P24" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q24" s="25" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="B25" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="O24" s="24" t="s">
+      <c r="C25" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="P24" s="28" t="s">
+      <c r="D25" s="21" t="s">
         <v>148</v>
-      </c>
-      <c r="Q24" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="R24" s="25" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="20" t="s">
-        <v>150</v>
-      </c>
-      <c r="B25" s="21" t="s">
-        <v>151</v>
-      </c>
-      <c r="C25" s="21" t="s">
-        <v>152</v>
-      </c>
-      <c r="D25" s="21" t="s">
-        <v>153</v>
       </c>
       <c r="E25" s="21"/>
       <c r="F25" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="G25" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="H25" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="I25" s="23" t="s">
         <v>28</v>
-      </c>
-      <c r="G25" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="H25" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="I25" s="23" t="s">
-        <v>29</v>
       </c>
       <c r="J25" s="21"/>
       <c r="K25" s="21"/>
       <c r="L25" s="21"/>
-      <c r="M25" s="21"/>
+      <c r="M25" s="21" t="s">
+        <v>175</v>
+      </c>
       <c r="N25" s="21" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="O25" s="28" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="P25" s="20">
         <v>0</v>
       </c>
-      <c r="Q25" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="R25" s="25" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" ht="72" x14ac:dyDescent="0.3">
+      <c r="Q25" s="25" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" ht="72" x14ac:dyDescent="0.3">
       <c r="A26" s="20" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C26" s="21" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D26" s="21" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="E26" s="21"/>
       <c r="F26" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="G26" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="G26" s="27" t="s">
-        <v>30</v>
-      </c>
       <c r="H26" s="27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I26" s="21" t="s">
+        <v>156</v>
+      </c>
+      <c r="J26" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="K26" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="L26" s="21"/>
+      <c r="M26" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="N26" s="21" t="s">
+        <v>157</v>
+      </c>
+      <c r="O26" s="28" t="s">
+        <v>158</v>
+      </c>
+      <c r="P26" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q26" s="28" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="B27" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="C27" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="D27" s="21" t="s">
         <v>161</v>
-      </c>
-      <c r="J26" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="K26" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="L26" s="21"/>
-      <c r="M26" s="21"/>
-      <c r="N26" s="21" t="s">
-        <v>162</v>
-      </c>
-      <c r="O26" s="28" t="s">
-        <v>163</v>
-      </c>
-      <c r="P26" s="24" t="s">
-        <v>136</v>
-      </c>
-      <c r="Q26" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="R26" s="28" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="20" t="s">
-        <v>157</v>
-      </c>
-      <c r="B27" s="21" t="s">
-        <v>158</v>
-      </c>
-      <c r="C27" s="21" t="s">
-        <v>165</v>
-      </c>
-      <c r="D27" s="21" t="s">
-        <v>166</v>
       </c>
       <c r="E27" s="21"/>
       <c r="F27" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G27" s="22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H27" s="21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I27" s="21" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="J27" s="21"/>
       <c r="K27" s="21"/>
       <c r="L27" s="21"/>
-      <c r="M27" s="21"/>
+      <c r="M27" s="21" t="s">
+        <v>177</v>
+      </c>
       <c r="N27" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="O27" s="28" t="s">
+        <v>163</v>
+      </c>
+      <c r="P27" s="30" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q27" s="25" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A28" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="B28" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="O27" s="28" t="s">
+      <c r="C28" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="P27" s="30" t="s">
+      <c r="D28" s="21" t="s">
         <v>169</v>
-      </c>
-      <c r="Q27" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="R27" s="25" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A28" s="20" t="s">
-        <v>171</v>
-      </c>
-      <c r="B28" s="21" t="s">
-        <v>172</v>
-      </c>
-      <c r="C28" s="21" t="s">
-        <v>173</v>
-      </c>
-      <c r="D28" s="21" t="s">
-        <v>174</v>
       </c>
       <c r="E28" s="21"/>
       <c r="F28" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G28" s="27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H28" s="27" t="s">
-        <v>45</v>
+        <v>181</v>
       </c>
       <c r="I28" s="27" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="J28" s="21"/>
       <c r="K28" s="21"/>
       <c r="L28" s="21"/>
-      <c r="M28" s="21"/>
+      <c r="M28" s="21" t="s">
+        <v>185</v>
+      </c>
       <c r="N28" s="21"/>
       <c r="P28" s="20"/>
-      <c r="Q28" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="R28" s="25" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="Q28" s="25" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A29" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="B29" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="C29" s="21" t="s">
         <v>171</v>
       </c>
-      <c r="B29" s="21" t="s">
+      <c r="D29" s="21" t="s">
         <v>172</v>
-      </c>
-      <c r="C29" s="21" t="s">
-        <v>176</v>
-      </c>
-      <c r="D29" s="21" t="s">
-        <v>177</v>
       </c>
       <c r="E29" s="21"/>
       <c r="F29" s="27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G29" s="27" t="s">
-        <v>45</v>
+        <v>181</v>
       </c>
       <c r="H29" s="27" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="I29" s="27" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="J29" s="21"/>
       <c r="K29" s="21"/>
       <c r="L29" s="21"/>
-      <c r="M29" s="21"/>
+      <c r="M29" s="21" t="s">
+        <v>186</v>
+      </c>
       <c r="N29" s="21"/>
       <c r="P29" s="20"/>
-      <c r="Q29" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="R29" s="25" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="Q29" s="25" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="C30" s="21"/>
       <c r="D30" s="21"/>
       <c r="E30" s="21"/>
@@ -2393,9 +2397,8 @@
       <c r="J30" s="21"/>
       <c r="K30" s="21"/>
       <c r="L30" s="21"/>
-      <c r="M30"/>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="C31" s="21"/>
       <c r="D31" s="21"/>
       <c r="E31" s="21"/>
@@ -2406,9 +2409,8 @@
       <c r="J31" s="21"/>
       <c r="K31" s="21"/>
       <c r="L31" s="21"/>
-      <c r="M31"/>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="C32" s="21"/>
       <c r="D32" s="21"/>
       <c r="E32" s="21"/>
@@ -2419,7 +2421,6 @@
       <c r="J32" s="21"/>
       <c r="K32" s="21"/>
       <c r="L32" s="21"/>
-      <c r="M32"/>
     </row>
     <row r="33" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C33" s="21"/>
@@ -2432,7 +2433,6 @@
       <c r="J33" s="21"/>
       <c r="K33" s="21"/>
       <c r="L33" s="21"/>
-      <c r="M33"/>
       <c r="N33" s="21"/>
     </row>
     <row r="34" spans="3:14" x14ac:dyDescent="0.3">
@@ -2446,7 +2446,6 @@
       <c r="J34" s="21"/>
       <c r="K34" s="21"/>
       <c r="L34" s="21"/>
-      <c r="M34"/>
     </row>
     <row r="35" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C35" s="21"/>
@@ -2459,7 +2458,6 @@
       <c r="J35" s="21"/>
       <c r="K35" s="21"/>
       <c r="L35" s="21"/>
-      <c r="M35"/>
     </row>
     <row r="36" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C36" s="21"/>
@@ -2472,7 +2470,6 @@
       <c r="J36" s="21"/>
       <c r="K36" s="21"/>
       <c r="L36" s="21"/>
-      <c r="M36"/>
     </row>
     <row r="37" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C37" s="21"/>
@@ -2485,7 +2482,6 @@
       <c r="J37" s="21"/>
       <c r="K37" s="21"/>
       <c r="L37" s="21"/>
-      <c r="M37"/>
     </row>
     <row r="38" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C38" s="21"/>
@@ -2498,7 +2494,6 @@
       <c r="J38" s="21"/>
       <c r="K38" s="21"/>
       <c r="L38" s="21"/>
-      <c r="M38"/>
     </row>
     <row r="39" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C39" s="21"/>
@@ -2553,11 +2548,10 @@
       <c r="M42" s="21"/>
     </row>
   </sheetData>
-  <autoFilter ref="A7:Q7" xr:uid="{996DE33A-D382-4857-9FF7-927B0A9B94CC}">
+  <autoFilter ref="A7:P7" xr:uid="{996DE33A-D382-4857-9FF7-927B0A9B94CC}">
     <filterColumn colId="14" showButton="0"/>
   </autoFilter>
-  <mergeCells count="8">
-    <mergeCell ref="Q6:R6"/>
+  <mergeCells count="7">
     <mergeCell ref="O7:P7"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="G1:L1"/>
@@ -2582,28 +2576,28 @@
     <hyperlink ref="P26" r:id="rId13" xr:uid="{B25F411D-D526-4327-BD0B-37E4CC13944F}"/>
     <hyperlink ref="O27" r:id="rId14" xr:uid="{3E17E50B-CBC0-44D1-97CB-FFFF7655B4C4}"/>
     <hyperlink ref="P27" r:id="rId15" xr:uid="{46A5C0C5-57A0-4A5A-9C82-B7E70C3B3B4C}"/>
-    <hyperlink ref="R8" r:id="rId16" xr:uid="{1BCFC2F6-9233-4ED2-90E0-1D5108F7A1E6}"/>
-    <hyperlink ref="R26" r:id="rId17" xr:uid="{8030B39F-01D8-4AA3-A11A-F8E97299759B}"/>
-    <hyperlink ref="R27" r:id="rId18" xr:uid="{05F01153-1E2C-449E-8812-4205A687871C}"/>
-    <hyperlink ref="R11" r:id="rId19" xr:uid="{790529B1-C5AD-4142-9BCE-25599DDFCFB0}"/>
-    <hyperlink ref="R19" r:id="rId20" xr:uid="{F6EFC093-9BDE-40BF-A38C-E26ECBE4848D}"/>
-    <hyperlink ref="R13" r:id="rId21" xr:uid="{0C15A771-1389-413E-9A8A-2D3D2225D5F7}"/>
-    <hyperlink ref="R18" r:id="rId22" xr:uid="{207CB203-B5D5-4D0D-8ACF-5A9FC7307BD3}"/>
-    <hyperlink ref="R14" r:id="rId23" xr:uid="{EFCDE6EA-6533-4C97-A38F-A882E2F5BC8B}"/>
-    <hyperlink ref="R15" r:id="rId24" xr:uid="{661759F1-5914-40A2-A766-B1924D0131A3}"/>
-    <hyperlink ref="R16" r:id="rId25" xr:uid="{E517FBE4-97AC-4847-A1C6-BFC6AA2E5CAE}"/>
-    <hyperlink ref="R17" r:id="rId26" xr:uid="{D67D0E5D-BD89-46EB-8A79-D61991256C04}"/>
-    <hyperlink ref="R20" r:id="rId27" xr:uid="{F2B19C62-90EE-4B7C-A1B9-2910528AE585}"/>
-    <hyperlink ref="R21" r:id="rId28" xr:uid="{9DBE5445-7F15-4EB4-B5A8-970CED0CA518}"/>
-    <hyperlink ref="R22" r:id="rId29" xr:uid="{A930C62D-D61E-4AEE-8693-BDBFAA61D6E3}"/>
-    <hyperlink ref="R23" r:id="rId30" xr:uid="{8B8308CE-99BC-469E-81C1-516BDF860524}"/>
-    <hyperlink ref="R24" r:id="rId31" xr:uid="{A972AA68-3BE2-43B9-A406-BD8D38B98BB5}"/>
-    <hyperlink ref="R25" r:id="rId32" xr:uid="{BB1CB586-031A-441C-AB3F-46F36A19698F}"/>
-    <hyperlink ref="R29" r:id="rId33" xr:uid="{2071A5AD-68CD-4A26-9930-C4DC9FBD9577}"/>
-    <hyperlink ref="R28" r:id="rId34" xr:uid="{EBFCE2EF-9D8F-4B92-94E4-267D34832233}"/>
-    <hyperlink ref="R9" r:id="rId35" xr:uid="{F47EDC67-7ED2-48A6-8B42-4F2E2DE048D5}"/>
-    <hyperlink ref="R10" r:id="rId36" xr:uid="{DE5B43A0-6310-4BE3-BAA5-F2C4F8B3464C}"/>
-    <hyperlink ref="R12" r:id="rId37" xr:uid="{1A8481D1-325B-4452-84A5-BE59B616E374}"/>
+    <hyperlink ref="Q8" r:id="rId16" xr:uid="{1BCFC2F6-9233-4ED2-90E0-1D5108F7A1E6}"/>
+    <hyperlink ref="Q26" r:id="rId17" xr:uid="{8030B39F-01D8-4AA3-A11A-F8E97299759B}"/>
+    <hyperlink ref="Q27" r:id="rId18" xr:uid="{05F01153-1E2C-449E-8812-4205A687871C}"/>
+    <hyperlink ref="Q11" r:id="rId19" xr:uid="{790529B1-C5AD-4142-9BCE-25599DDFCFB0}"/>
+    <hyperlink ref="Q19" r:id="rId20" xr:uid="{F6EFC093-9BDE-40BF-A38C-E26ECBE4848D}"/>
+    <hyperlink ref="Q13" r:id="rId21" xr:uid="{0C15A771-1389-413E-9A8A-2D3D2225D5F7}"/>
+    <hyperlink ref="Q18" r:id="rId22" xr:uid="{207CB203-B5D5-4D0D-8ACF-5A9FC7307BD3}"/>
+    <hyperlink ref="Q14" r:id="rId23" xr:uid="{EFCDE6EA-6533-4C97-A38F-A882E2F5BC8B}"/>
+    <hyperlink ref="Q15" r:id="rId24" xr:uid="{661759F1-5914-40A2-A766-B1924D0131A3}"/>
+    <hyperlink ref="Q16" r:id="rId25" xr:uid="{E517FBE4-97AC-4847-A1C6-BFC6AA2E5CAE}"/>
+    <hyperlink ref="Q17" r:id="rId26" xr:uid="{D67D0E5D-BD89-46EB-8A79-D61991256C04}"/>
+    <hyperlink ref="Q20" r:id="rId27" xr:uid="{F2B19C62-90EE-4B7C-A1B9-2910528AE585}"/>
+    <hyperlink ref="Q21" r:id="rId28" xr:uid="{9DBE5445-7F15-4EB4-B5A8-970CED0CA518}"/>
+    <hyperlink ref="Q22" r:id="rId29" xr:uid="{A930C62D-D61E-4AEE-8693-BDBFAA61D6E3}"/>
+    <hyperlink ref="Q23" r:id="rId30" xr:uid="{8B8308CE-99BC-469E-81C1-516BDF860524}"/>
+    <hyperlink ref="Q24" r:id="rId31" xr:uid="{A972AA68-3BE2-43B9-A406-BD8D38B98BB5}"/>
+    <hyperlink ref="Q25" r:id="rId32" xr:uid="{BB1CB586-031A-441C-AB3F-46F36A19698F}"/>
+    <hyperlink ref="Q29" r:id="rId33" xr:uid="{2071A5AD-68CD-4A26-9930-C4DC9FBD9577}"/>
+    <hyperlink ref="Q28" r:id="rId34" xr:uid="{EBFCE2EF-9D8F-4B92-94E4-267D34832233}"/>
+    <hyperlink ref="Q9" r:id="rId35" xr:uid="{F47EDC67-7ED2-48A6-8B42-4F2E2DE048D5}"/>
+    <hyperlink ref="Q10" r:id="rId36" xr:uid="{DE5B43A0-6310-4BE3-BAA5-F2C4F8B3464C}"/>
+    <hyperlink ref="Q12" r:id="rId37" xr:uid="{1A8481D1-325B-4452-84A5-BE59B616E374}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>